<commit_message>
added results on test-set for all models
</commit_message>
<xml_diff>
--- a/evaluation/batch/refine/tuning_2.xlsx
+++ b/evaluation/batch/refine/tuning_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\falco\Desktop\NeuralNetwork-library\evaluation\batch\refine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB8E4A4-BA4A-48AD-BB19-ADDAD248EB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2A8BD6-D2E4-4C8D-B9D9-D28D11F39A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +59,90 @@
   </si>
   <si>
     <t>f1-score_val</t>
+  </si>
+  <si>
+    <t>acc_test</t>
+  </si>
+  <si>
+    <t>0.9676</t>
+  </si>
+  <si>
+    <t>0.9521</t>
+  </si>
+  <si>
+    <t>0.845</t>
+  </si>
+  <si>
+    <t>0.9698</t>
+  </si>
+  <si>
+    <t>0.9685</t>
+  </si>
+  <si>
+    <t>0.9403</t>
+  </si>
+  <si>
+    <t>0.9548</t>
+  </si>
+  <si>
+    <t>0.9601</t>
+  </si>
+  <si>
+    <t>0.9486</t>
+  </si>
+  <si>
+    <t>0.9453</t>
+  </si>
+  <si>
+    <t>0.9479</t>
+  </si>
+  <si>
+    <t>0.8978</t>
+  </si>
+  <si>
+    <t>0.9678</t>
+  </si>
+  <si>
+    <t>0.9692</t>
+  </si>
+  <si>
+    <t>0.9394</t>
+  </si>
+  <si>
+    <t>0.9567</t>
+  </si>
+  <si>
+    <t>0.9626</t>
+  </si>
+  <si>
+    <t>0.9492</t>
+  </si>
+  <si>
+    <t>0.9604</t>
+  </si>
+  <si>
+    <t>0.9231</t>
+  </si>
+  <si>
+    <t>0.7946</t>
+  </si>
+  <si>
+    <t>0.9665</t>
+  </si>
+  <si>
+    <t>0.9707</t>
+  </si>
+  <si>
+    <t>0.9146</t>
+  </si>
+  <si>
+    <t>0.9569</t>
+  </si>
+  <si>
+    <t>0.9628</t>
+  </si>
+  <si>
+    <t>0.9498</t>
   </si>
 </sst>
 </file>
@@ -476,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,15 +574,16 @@
     <col min="4" max="4" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="8" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,28 +603,31 @@
         <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>60</v>
       </c>
@@ -558,29 +646,32 @@
       <c r="F2" s="8">
         <v>0.96158333333333335</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8">
         <v>2075.7619743310938</v>
       </c>
-      <c r="H2" s="8">
+      <c r="I2" s="8">
         <v>1493.1515621419569</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>428</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>413</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>244.71</v>
       </c>
-      <c r="L2" s="8">
+      <c r="M2" s="8">
         <v>0.99008700456324716</v>
       </c>
-      <c r="M2" s="8">
+      <c r="N2" s="8">
         <v>0.96102148748394389</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>61</v>
       </c>
@@ -599,29 +690,32 @@
       <c r="F3" s="8">
         <v>0.94766666666666666</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="8">
         <v>4256.7740309690926</v>
       </c>
-      <c r="H3" s="8">
+      <c r="I3" s="8">
         <v>2227.1434777540021</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>434</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <v>419</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <v>305.12</v>
       </c>
-      <c r="L3" s="8">
+      <c r="M3" s="8">
         <v>0.9751915495187079</v>
       </c>
-      <c r="M3" s="8">
+      <c r="N3" s="8">
         <v>0.94686394368227644</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>62</v>
       </c>
@@ -640,29 +734,32 @@
       <c r="F4" s="8">
         <v>0.84116666666666662</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="8">
         <v>31024.2441712738</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I4" s="8">
         <v>7666.4982363068502</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="4">
         <v>33</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>18</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>27.53</v>
       </c>
-      <c r="L4" s="8">
+      <c r="M4" s="8">
         <v>0.83859669818229732</v>
       </c>
-      <c r="M4" s="8">
+      <c r="N4" s="8">
         <v>0.83747050953088409</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>63</v>
       </c>
@@ -681,27 +778,30 @@
       <c r="F5" s="9">
         <v>0.96866666666666668</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="9">
         <v>2045.998920517495</v>
       </c>
-      <c r="H5" s="9">
+      <c r="I5" s="9">
         <v>1268.533407503531</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
         <v>499</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <v>374.58</v>
       </c>
-      <c r="L5" s="9">
+      <c r="M5" s="9">
         <v>0.99028530346682275</v>
       </c>
-      <c r="M5" s="9">
+      <c r="N5" s="9">
         <v>0.96829258151756803</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>64</v>
       </c>
@@ -720,26 +820,29 @@
       <c r="F6" s="8">
         <v>0.96691666666666665</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="8">
         <v>1538.499989795213</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I6" s="8">
         <v>1336.9097108440949</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>485</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>265.57</v>
       </c>
-      <c r="L6" s="8">
+      <c r="M6" s="8">
         <v>0.99404138697923194</v>
       </c>
-      <c r="M6" s="8">
+      <c r="N6" s="8">
         <v>0.96646686120521308</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>65</v>
       </c>
@@ -758,29 +861,32 @@
       <c r="F7" s="8">
         <v>0.93774999999999997</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="8">
         <v>5888.4497279700036</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>3441.6599632144448</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>320</v>
       </c>
-      <c r="J7" s="4">
+      <c r="K7" s="4">
         <v>305</v>
       </c>
-      <c r="K7" s="4">
+      <c r="L7" s="4">
         <v>173.28</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="8">
         <v>0.9647927526342196</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>0.93681505762087025</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>66</v>
       </c>
@@ -799,26 +905,29 @@
       <c r="F8" s="8">
         <v>0.95374999999999999</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="8">
         <v>6537.0709854355237</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>1919.095464593996</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <v>499</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <v>263.58999999999997</v>
       </c>
-      <c r="L8" s="8">
+      <c r="M8" s="8">
         <v>0.9618150577542508</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>0.95307451293418377</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>67</v>
       </c>
@@ -837,26 +946,29 @@
       <c r="F9" s="8">
         <v>0.95808333333333329</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="8">
         <v>5322.3816022475921</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I9" s="8">
         <v>1706.7441079996131</v>
       </c>
-      <c r="J9" s="4">
+      <c r="K9" s="4">
         <v>499</v>
       </c>
-      <c r="K9" s="4">
+      <c r="L9" s="4">
         <v>261.10000000000002</v>
       </c>
-      <c r="L9" s="8">
+      <c r="M9" s="8">
         <v>0.9695626560176841</v>
       </c>
-      <c r="M9" s="8">
+      <c r="N9" s="8">
         <v>0.95742519798610992</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>68</v>
       </c>
@@ -875,26 +987,29 @@
       <c r="F10" s="8">
         <v>0.94491666666666663</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="8">
         <v>4206.8785369342841</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <v>2773.0671744613041</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>499</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <v>263.60000000000002</v>
       </c>
-      <c r="L10" s="8">
+      <c r="M10" s="8">
         <v>0.97485885288214613</v>
       </c>
-      <c r="M10" s="8">
+      <c r="N10" s="8">
         <v>0.94394394378017688</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>69</v>
       </c>
@@ -913,29 +1028,32 @@
       <c r="F11" s="8">
         <v>0.93925000000000003</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="8">
         <v>6422.6540966890007</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="8">
         <v>2407.0975789361601</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>312</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <v>297</v>
       </c>
-      <c r="K11" s="4">
+      <c r="L11" s="4">
         <v>179.2</v>
       </c>
-      <c r="L11" s="8">
+      <c r="M11" s="8">
         <v>0.96257661285206919</v>
       </c>
-      <c r="M11" s="8">
+      <c r="N11" s="8">
         <v>0.93809551765043508</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>70</v>
       </c>
@@ -954,29 +1072,32 @@
       <c r="F12" s="8">
         <v>0.94533333333333336</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="8">
         <v>4936.0554019796673</v>
       </c>
-      <c r="H12" s="8">
+      <c r="I12" s="8">
         <v>2359.0292397750532</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="4">
         <v>372</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <v>357</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="4">
         <v>213.02</v>
       </c>
-      <c r="L12" s="8">
+      <c r="M12" s="8">
         <v>0.97211160210043257</v>
       </c>
-      <c r="M12" s="8">
+      <c r="N12" s="8">
         <v>0.94465745000503676</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>71</v>
       </c>
@@ -995,29 +1116,32 @@
       <c r="F13" s="8">
         <v>0.89500000000000002</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="8">
         <v>18392.599286013668</v>
       </c>
-      <c r="H13" s="8">
+      <c r="I13" s="8">
         <v>5572.5249913176367</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="4">
         <v>173</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <v>158</v>
       </c>
-      <c r="K13" s="4">
+      <c r="L13" s="4">
         <v>117.49</v>
       </c>
-      <c r="L13" s="8">
+      <c r="M13" s="8">
         <v>0.90257433800233533</v>
       </c>
-      <c r="M13" s="8">
+      <c r="N13" s="8">
         <v>0.89361624947990337</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>72</v>
       </c>
@@ -1036,26 +1160,29 @@
       <c r="F14" s="8">
         <v>0.96450000000000002</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="8">
         <v>2204.3266706138352</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="8">
         <v>1364.7825306059181</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <v>499</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <v>300.95999999999998</v>
       </c>
-      <c r="L14" s="8">
+      <c r="M14" s="8">
         <v>0.98924577096744082</v>
       </c>
-      <c r="M14" s="8">
+      <c r="N14" s="8">
         <v>0.96393816173434177</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>73</v>
       </c>
@@ -1074,29 +1201,32 @@
       <c r="F15" s="10">
         <v>0.96499999999999997</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="10">
         <v>1682.880188338579</v>
       </c>
-      <c r="H15" s="10">
+      <c r="I15" s="10">
         <v>1431.8487155178409</v>
       </c>
-      <c r="I15" s="6">
+      <c r="J15" s="6">
         <v>434</v>
       </c>
-      <c r="J15" s="6">
+      <c r="K15" s="6">
         <v>419</v>
       </c>
-      <c r="K15" s="6">
+      <c r="L15" s="6">
         <v>245.98</v>
       </c>
-      <c r="L15" s="10">
+      <c r="M15" s="10">
         <v>0.99345547220989694</v>
       </c>
-      <c r="M15" s="10">
+      <c r="N15" s="10">
         <v>0.96449057465403487</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>74</v>
       </c>
@@ -1115,29 +1245,32 @@
       <c r="F16" s="8">
         <v>0.93558333333333332</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="8">
         <v>6573.9486935451077</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="8">
         <v>3618.320307242735</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="4">
         <v>274</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <v>259</v>
       </c>
-      <c r="K16" s="4">
+      <c r="L16" s="4">
         <v>153.85</v>
       </c>
-      <c r="L16" s="8">
+      <c r="M16" s="8">
         <v>0.96068171225915289</v>
       </c>
-      <c r="M16" s="8">
+      <c r="N16" s="8">
         <v>0.93455822147264556</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>75</v>
       </c>
@@ -1156,26 +1289,29 @@
       <c r="F17" s="8">
         <v>0.95150000000000001</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="8">
         <v>6630.8066458993198</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I17" s="8">
         <v>1962.7934084846611</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>499</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <v>281.31</v>
       </c>
-      <c r="L17" s="8">
+      <c r="M17" s="8">
         <v>0.96149600504568133</v>
       </c>
-      <c r="M17" s="8">
+      <c r="N17" s="8">
         <v>0.9507364355757788</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>76</v>
       </c>
@@ -1194,26 +1330,29 @@
       <c r="F18" s="8">
         <v>0.95858333333333334</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="8">
         <v>5087.3263583453836</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="8">
         <v>1655.5040091298481</v>
       </c>
-      <c r="J18" s="4">
+      <c r="K18" s="4">
         <v>499</v>
       </c>
-      <c r="K18" s="4">
+      <c r="L18" s="4">
         <v>280.06</v>
       </c>
-      <c r="L18" s="8">
+      <c r="M18" s="8">
         <v>0.97063009521035293</v>
       </c>
-      <c r="M18" s="8">
+      <c r="N18" s="8">
         <v>0.95795185671693039</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>77</v>
       </c>
@@ -1232,26 +1371,29 @@
       <c r="F19" s="8">
         <v>0.94491666666666663</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="8">
         <v>3916.7224779184448</v>
       </c>
-      <c r="H19" s="8">
+      <c r="I19" s="8">
         <v>2656.749649123351</v>
       </c>
-      <c r="J19" s="4">
+      <c r="K19" s="4">
         <v>499</v>
       </c>
-      <c r="K19" s="4">
+      <c r="L19" s="4">
         <v>286.14</v>
       </c>
-      <c r="L19" s="8">
+      <c r="M19" s="8">
         <v>0.97699013364912202</v>
       </c>
-      <c r="M19" s="8">
+      <c r="N19" s="8">
         <v>0.94399982755929945</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>78</v>
       </c>
@@ -1270,29 +1412,32 @@
       <c r="F20" s="8">
         <v>0.95691666666666664</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="8">
         <v>3090.0871996014662</v>
       </c>
-      <c r="H20" s="8">
+      <c r="I20" s="8">
         <v>1777.7045273983281</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>462</v>
       </c>
-      <c r="J20" s="4">
+      <c r="K20" s="4">
         <v>447</v>
       </c>
-      <c r="K20" s="4">
+      <c r="L20" s="4">
         <v>263.89999999999998</v>
       </c>
-      <c r="L20" s="8">
+      <c r="M20" s="8">
         <v>0.98443016570368758</v>
       </c>
-      <c r="M20" s="8">
+      <c r="N20" s="8">
         <v>0.95619985823164588</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>79</v>
       </c>
@@ -1311,29 +1456,32 @@
       <c r="F21" s="8">
         <v>0.91874999999999996</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="8">
         <v>10961.24002584256</v>
       </c>
-      <c r="H21" s="8">
+      <c r="I21" s="8">
         <v>3382.809623980188</v>
       </c>
-      <c r="I21" s="4">
+      <c r="J21" s="4">
         <v>211</v>
       </c>
-      <c r="J21" s="4">
+      <c r="K21" s="4">
         <v>196</v>
       </c>
-      <c r="K21" s="4">
+      <c r="L21" s="4">
         <v>118.65</v>
       </c>
-      <c r="L21" s="8">
+      <c r="M21" s="8">
         <v>0.93651638626544642</v>
       </c>
-      <c r="M21" s="8">
+      <c r="N21" s="8">
         <v>0.91719562591417458</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>80</v>
       </c>
@@ -1352,29 +1500,32 @@
       <c r="F22" s="8">
         <v>0.78716666666666668</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="8">
         <v>41599.778807339208</v>
       </c>
-      <c r="H22" s="8">
+      <c r="I22" s="8">
         <v>10368.56586639906</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <v>41</v>
       </c>
-      <c r="J22" s="4">
+      <c r="K22" s="4">
         <v>26</v>
       </c>
-      <c r="K22" s="4">
+      <c r="L22" s="4">
         <v>24.74</v>
       </c>
-      <c r="L22" s="8">
+      <c r="M22" s="8">
         <v>0.77324638191252826</v>
       </c>
-      <c r="M22" s="8">
+      <c r="N22" s="8">
         <v>0.77152543366693671</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>81</v>
       </c>
@@ -1393,26 +1544,29 @@
       <c r="F23" s="8">
         <v>0.96475</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="8">
         <v>2433.0146448160172</v>
       </c>
-      <c r="H23" s="8">
+      <c r="I23" s="8">
         <v>1373.2498408399331</v>
       </c>
-      <c r="J23" s="4">
+      <c r="K23" s="4">
         <v>499</v>
       </c>
-      <c r="K23" s="4">
+      <c r="L23" s="4">
         <v>278.25</v>
       </c>
-      <c r="L23" s="8">
+      <c r="M23" s="8">
         <v>0.98850448106174782</v>
       </c>
-      <c r="M23" s="8">
+      <c r="N23" s="8">
         <v>0.96412736798181287</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>82</v>
       </c>
@@ -1431,29 +1585,32 @@
       <c r="F24" s="8">
         <v>0.96733333333333338</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="8">
         <v>1516.946984169012</v>
       </c>
-      <c r="H24" s="8">
+      <c r="I24" s="8">
         <v>1333.239739817117</v>
       </c>
-      <c r="I24" s="4">
+      <c r="J24" s="4">
         <v>486</v>
       </c>
-      <c r="J24" s="4">
+      <c r="K24" s="4">
         <v>471</v>
       </c>
-      <c r="K24" s="4">
+      <c r="L24" s="4">
         <v>270.87</v>
       </c>
-      <c r="L24" s="8">
+      <c r="M24" s="8">
         <v>0.99412273337488277</v>
       </c>
-      <c r="M24" s="8">
+      <c r="N24" s="8">
         <v>0.96691575382234107</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>83</v>
       </c>
@@ -1472,29 +1629,32 @@
       <c r="F25" s="8">
         <v>0.90483333333333338</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="8">
         <v>20611.4904912081</v>
       </c>
-      <c r="H25" s="8">
+      <c r="I25" s="8">
         <v>5855.0921508920901</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>64</v>
       </c>
-      <c r="J25" s="4">
+      <c r="K25" s="4">
         <v>49</v>
       </c>
-      <c r="K25" s="4">
+      <c r="L25" s="4">
         <v>37.549999999999997</v>
       </c>
-      <c r="L25" s="8">
+      <c r="M25" s="8">
         <v>0.91096331636654015</v>
       </c>
-      <c r="M25" s="8">
+      <c r="N25" s="8">
         <v>0.90310571067305823</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>84</v>
       </c>
@@ -1513,26 +1673,29 @@
       <c r="F26" s="8">
         <v>0.95533333333333337</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G26" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="8">
         <v>6341.8511093499455</v>
       </c>
-      <c r="H26" s="8">
+      <c r="I26" s="8">
         <v>1855.5055666923561</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>499</v>
       </c>
-      <c r="K26" s="4">
+      <c r="L26" s="4">
         <v>280.3</v>
       </c>
-      <c r="L26" s="8">
+      <c r="M26" s="8">
         <v>0.96265562267706417</v>
       </c>
-      <c r="M26" s="8">
+      <c r="N26" s="8">
         <v>0.95465918713577747</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>85</v>
       </c>
@@ -1551,26 +1714,29 @@
       <c r="F27" s="8">
         <v>0.96166666666666667</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="8">
         <v>4839.0507185174656</v>
       </c>
-      <c r="H27" s="8">
+      <c r="I27" s="8">
         <v>1582.94765088339</v>
       </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
         <v>499</v>
       </c>
-      <c r="K27" s="4">
+      <c r="L27" s="4">
         <v>277.64999999999998</v>
       </c>
-      <c r="L27" s="8">
+      <c r="M27" s="8">
         <v>0.97241247326314917</v>
       </c>
-      <c r="M27" s="8">
+      <c r="N27" s="8">
         <v>0.9611398530151174</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>86</v>
       </c>
@@ -1589,22 +1755,25 @@
       <c r="F28" s="8">
         <v>0.94616666666666671</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" t="s">
+        <v>40</v>
+      </c>
+      <c r="H28" s="8">
         <v>3905.0975115682081</v>
       </c>
-      <c r="H28" s="8">
+      <c r="I28" s="8">
         <v>2621.2787347047029</v>
       </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
         <v>499</v>
       </c>
-      <c r="K28" s="4">
+      <c r="L28" s="4">
         <v>278.02999999999997</v>
       </c>
-      <c r="L28" s="8">
+      <c r="M28" s="8">
         <v>0.97750771924559066</v>
       </c>
-      <c r="M28" s="8">
+      <c r="N28" s="8">
         <v>0.94529757914191193</v>
       </c>
     </row>

</xml_diff>